<commit_message>
Took ownership of issues 1 through 3
</commit_message>
<xml_diff>
--- a/Documentation/issue tracker.xlsx
+++ b/Documentation/issue tracker.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>ISSUE TRACKER</t>
   </si>
@@ -51,9 +51,6 @@
     <t>DATE CLOSED</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t xml:space="preserve">ISSUE# </t>
   </si>
   <si>
@@ -94,6 +91,12 @@
   </si>
   <si>
     <t>Add an "undefined" check and use place holder text instead.  Mng-feed.php</t>
+  </si>
+  <si>
+    <t>Rob Sims</t>
+  </si>
+  <si>
+    <t>In Process</t>
   </si>
 </sst>
 </file>
@@ -242,15 +245,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -293,6 +287,15 @@
         <bottom/>
       </border>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -1297,11 +1300,11 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="IssueTrackerTbl" displayName="IssueTrackerTbl" ref="B2:J5">
   <tableColumns count="9">
-    <tableColumn id="1" name="ISSUE# " totalsRowLabel="Total" totalsRowDxfId="4" dataCellStyle="Issue Description"/>
+    <tableColumn id="1" name="ISSUE# " totalsRowLabel="Total" totalsRowDxfId="3" dataCellStyle="Issue Description"/>
     <tableColumn id="2" name="DATE OPENED" dataCellStyle="Date"/>
-    <tableColumn id="3" name="PRIORITY" dataDxfId="3"/>
-    <tableColumn id="9" name="ISSUE DESCRIPTION" dataDxfId="2"/>
-    <tableColumn id="11" name="INITIAL ANALYSIS" dataDxfId="1"/>
+    <tableColumn id="3" name="PRIORITY" dataDxfId="2"/>
+    <tableColumn id="9" name="ISSUE DESCRIPTION" dataDxfId="1"/>
+    <tableColumn id="11" name="INITIAL ANALYSIS" dataDxfId="0"/>
     <tableColumn id="4" name="ASSIGNED"/>
     <tableColumn id="5" name="STATUS"/>
     <tableColumn id="6" name="RESOLUTION"/>
@@ -1525,7 +1528,7 @@
   <dimension ref="B1:L6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1556,7 +1559,7 @@
     </row>
     <row r="2" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
@@ -1565,10 +1568,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>3</v>
@@ -1583,7 +1586,7 @@
         <v>6</v>
       </c>
       <c r="L2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1597,19 +1600,21 @@
         <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="H3" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="6"/>
       <c r="L3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1623,19 +1628,21 @@
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="H4" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="6"/>
       <c r="L4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1649,29 +1656,31 @@
         <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="6"/>
       <c r="L5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>ROW()=LastRow</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Issues #1 through #3 fixed
</commit_message>
<xml_diff>
--- a/Documentation/issue tracker.xlsx
+++ b/Documentation/issue tracker.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>ISSUE TRACKER</t>
   </si>
@@ -96,7 +96,10 @@
     <t>Rob Sims</t>
   </si>
   <si>
-    <t>In Process</t>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>amended comments.php</t>
   </si>
 </sst>
 </file>
@@ -1528,7 +1531,7 @@
   <dimension ref="B1:L6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1611,8 +1614,12 @@
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="6"/>
+      <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="6">
+        <v>42818</v>
+      </c>
       <c r="L3" t="s">
         <v>10</v>
       </c>
@@ -1639,8 +1646,12 @@
       <c r="H4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="6"/>
+      <c r="I4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="6">
+        <v>42818</v>
+      </c>
       <c r="L4" t="s">
         <v>11</v>
       </c>
@@ -1667,8 +1678,12 @@
       <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="6"/>
+      <c r="I5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="6">
+        <v>42818</v>
+      </c>
       <c r="L5" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Issues 4 through 7 added.
</commit_message>
<xml_diff>
--- a/Documentation/issue tracker.xlsx
+++ b/Documentation/issue tracker.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box Sync\University\Semester two\RIA\Ass 1\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
@@ -18,7 +13,7 @@
     <definedName name="LastRow">MAX(ROW(IssueTrackerTbl[ISSUE'# ]))</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Issue Tracker'!$2:$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>ISSUE TRACKER</t>
   </si>
@@ -100,13 +95,37 @@
   </si>
   <si>
     <t>amended comments.php</t>
+  </si>
+  <si>
+    <t>Can view other peoples subscriptions by editing url directly (i.e. putting in a different userid).</t>
+  </si>
+  <si>
+    <t>Reconmend adding something like if ($_SESSION[userid] != $_GET[userid]) check on mysubscription.php</t>
+  </si>
+  <si>
+    <t>Show all feeds to any user that is logged in.</t>
+  </si>
+  <si>
+    <t>Userid superflous for feeds.php and comments.php now we have a separate My Subscriptions page.</t>
+  </si>
+  <si>
+    <t>Logo is not totally responsive</t>
+  </si>
+  <si>
+    <t>Check all Media Query breakpoints</t>
+  </si>
+  <si>
+    <t>Feed thumbs are not responsive</t>
+  </si>
+  <si>
+    <t>Make responsive through feeds.php and css - see comments'php for similar approach.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <b/>
       <sz val="9"/>
@@ -147,13 +166,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -192,7 +247,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -211,42 +266,108 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="4">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="9">
+    <cellStyle name="Bad" xfId="7" builtinId="27"/>
     <cellStyle name="Date" xfId="4"/>
+    <cellStyle name="Good" xfId="6" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Issue Description" xfId="5"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -331,10 +452,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Issue Tracker" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Issue Tracker" pivot="0" count="4">
-      <tableStyleElement type="headerRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="secondRowStripe" dxfId="6"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="secondRowStripe" dxfId="10"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1301,13 +1422,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="IssueTrackerTbl" displayName="IssueTrackerTbl" ref="B2:J5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="IssueTrackerTbl" displayName="IssueTrackerTbl" ref="B2:J9">
   <tableColumns count="9">
-    <tableColumn id="1" name="ISSUE# " totalsRowLabel="Total" totalsRowDxfId="3" dataCellStyle="Issue Description"/>
+    <tableColumn id="1" name="ISSUE# " totalsRowLabel="Total" totalsRowDxfId="7" dataCellStyle="Issue Description"/>
     <tableColumn id="2" name="DATE OPENED" dataCellStyle="Date"/>
-    <tableColumn id="3" name="PRIORITY" dataDxfId="2"/>
-    <tableColumn id="9" name="ISSUE DESCRIPTION" dataDxfId="1"/>
-    <tableColumn id="11" name="INITIAL ANALYSIS" dataDxfId="0"/>
+    <tableColumn id="3" name="PRIORITY" dataDxfId="6"/>
+    <tableColumn id="9" name="ISSUE DESCRIPTION" dataDxfId="5"/>
+    <tableColumn id="11" name="INITIAL ANALYSIS" dataDxfId="4"/>
     <tableColumn id="4" name="ASSIGNED"/>
     <tableColumn id="5" name="STATUS"/>
     <tableColumn id="6" name="RESOLUTION"/>
@@ -1517,7 +1638,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1528,22 +1649,22 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="B1:L6"/>
+  <dimension ref="B1:L9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.83203125" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="6" width="49.83203125" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="14.83203125" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="25.83203125" customWidth="1"/>
     <col min="12" max="12" width="56.5" customWidth="1"/>
   </cols>
@@ -1561,31 +1682,31 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="L2" t="s">
@@ -1593,31 +1714,31 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="7">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>42818</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>42818</v>
       </c>
       <c r="L3" t="s">
@@ -1625,31 +1746,31 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="7">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>41722</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>42818</v>
       </c>
       <c r="L4" t="s">
@@ -1657,31 +1778,31 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="7">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>42818</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>42818</v>
       </c>
       <c r="L5" t="s">
@@ -1689,18 +1810,100 @@
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="12">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10">
+        <v>42822</v>
+      </c>
+      <c r="D6" s="11">
+        <v>2</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="10"/>
       <c r="L6" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>42822</v>
+      </c>
+      <c r="D7" s="14">
+        <v>3</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9">
+        <v>42822</v>
+      </c>
+      <c r="D8" s="14">
+        <v>3</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9">
+        <v>42944</v>
+      </c>
+      <c r="D9" s="14">
+        <v>4</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="9"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="4" priority="1">
+  <conditionalFormatting sqref="B3:B9">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>ROW()=LastRow</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please input a status. Click Cancel to pick from some options." sqref="H3:H5">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please input a status. Click Cancel to pick from some options." sqref="H3:H9">
       <formula1>"Not Started,In Process,Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>